<commit_message>
Update LIDO attributionQualifier excel file
</commit_message>
<xml_diff>
--- a/DataValueClustering/experiments/exports/evaluation/xlido_attribution_qualifier_randomized_0_1000000_hierarchical_20210319-145730_ready.xlsx
+++ b/DataValueClustering/experiments/exports/evaluation/xlido_attribution_qualifier_randomized_0_1000000_hierarchical_20210319-145730_ready.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viola Wenz\Documents\Repositories\data-value-clustering\DataValueClustering\experiments\exports\evaluation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster_Original" sheetId="1" r:id="rId1"/>
     <sheet name="Cluster_Repr" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -227,8 +232,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,7 +259,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFGREY"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,15 +341,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -386,7 +399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -418,9 +431,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -452,6 +466,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -627,12 +642,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -659,7 +674,7 @@
     <col min="23" max="23" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -706,7 +721,7 @@
       </c>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -755,7 +770,7 @@
       </c>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -817,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
@@ -849,7 +864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
@@ -881,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
@@ -913,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
@@ -939,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
@@ -965,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
@@ -985,7 +1000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1005,7 +1020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1019,7 +1034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1033,7 +1048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1061,7 +1076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
         <v>15</v>
       </c>
@@ -1075,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="8:9">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1083,7 +1098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="8:9">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="5" t="s">
         <v>40</v>
       </c>
@@ -1091,7 +1106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="8:9">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="5" t="s">
         <v>41</v>
       </c>
@@ -1099,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="8:9">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="5" t="s">
         <v>42</v>
       </c>
@@ -1107,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="8:9">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="5" t="s">
         <v>43</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="8:9">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="5" t="s">
         <v>44</v>
       </c>
@@ -1123,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="8:9">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H23" s="5" t="s">
         <v>45</v>
       </c>
@@ -1135,8 +1150,8 @@
   <conditionalFormatting sqref="B3:X3">
     <cfRule type="dataBar" priority="12">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF63C384"/>
       </dataBar>
     </cfRule>
@@ -1144,8 +1159,8 @@
   <conditionalFormatting sqref="C4">
     <cfRule type="dataBar" priority="1">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1153,8 +1168,8 @@
   <conditionalFormatting sqref="E4:E17">
     <cfRule type="dataBar" priority="2">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1162,8 +1177,8 @@
   <conditionalFormatting sqref="G4:G12">
     <cfRule type="dataBar" priority="3">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1171,8 +1186,8 @@
   <conditionalFormatting sqref="I4:I24">
     <cfRule type="dataBar" priority="4">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1180,8 +1195,8 @@
   <conditionalFormatting sqref="K4:K8">
     <cfRule type="dataBar" priority="5">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1189,8 +1204,8 @@
   <conditionalFormatting sqref="M4:M10">
     <cfRule type="dataBar" priority="6">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1198,8 +1213,8 @@
   <conditionalFormatting sqref="O4:O5">
     <cfRule type="dataBar" priority="7">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1207,8 +1222,8 @@
   <conditionalFormatting sqref="Q4:Q5">
     <cfRule type="dataBar" priority="8">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1216,8 +1231,8 @@
   <conditionalFormatting sqref="S4:S5">
     <cfRule type="dataBar" priority="9">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1225,8 +1240,8 @@
   <conditionalFormatting sqref="U4:U5">
     <cfRule type="dataBar" priority="10">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1234,8 +1249,8 @@
   <conditionalFormatting sqref="W4:W5">
     <cfRule type="dataBar" priority="11">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1245,39 +1260,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
     <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" customWidth="1"/>
     <col min="11" max="11" width="6.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
     <col min="13" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="38.7109375" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" customWidth="1"/>
     <col min="17" max="17" width="6.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="30.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="30.7109375" customWidth="1"/>
     <col min="21" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+    <col min="22" max="22" width="47" customWidth="1"/>
     <col min="23" max="23" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1324,7 +1341,7 @@
       </c>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1390,7 @@
       </c>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
@@ -1422,7 +1439,7 @@
       </c>
       <c r="W4" s="4"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1516,7 +1533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1548,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1580,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1606,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1632,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1666,7 +1683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1680,7 +1697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1694,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1708,7 +1725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H16" s="5" t="s">
         <v>38</v>
       </c>
@@ -1716,7 +1733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="8:9">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="5" t="s">
         <v>37</v>
       </c>
@@ -1724,7 +1741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="8:9">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="5" t="s">
         <v>40</v>
       </c>
@@ -1732,7 +1749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="8:9">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="5" t="s">
         <v>41</v>
       </c>
@@ -1740,7 +1757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="8:9">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="5" t="s">
         <v>42</v>
       </c>
@@ -1748,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="8:9">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="5" t="s">
         <v>43</v>
       </c>
@@ -1756,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="8:9">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="5" t="s">
         <v>45</v>
       </c>
@@ -1768,8 +1785,8 @@
   <conditionalFormatting sqref="B3:X3">
     <cfRule type="dataBar" priority="12">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF63C384"/>
       </dataBar>
     </cfRule>
@@ -1777,8 +1794,8 @@
   <conditionalFormatting sqref="B4:X4">
     <cfRule type="dataBar" priority="13">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FFC3C365"/>
       </dataBar>
     </cfRule>
@@ -1786,8 +1803,8 @@
   <conditionalFormatting sqref="C4:C5">
     <cfRule type="dataBar" priority="1">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1795,8 +1812,8 @@
   <conditionalFormatting sqref="E5:E16">
     <cfRule type="dataBar" priority="2">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1804,8 +1821,8 @@
   <conditionalFormatting sqref="G5:G12">
     <cfRule type="dataBar" priority="3">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1813,8 +1830,8 @@
   <conditionalFormatting sqref="I5:I23">
     <cfRule type="dataBar" priority="4">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1822,8 +1839,8 @@
   <conditionalFormatting sqref="K5:K9">
     <cfRule type="dataBar" priority="5">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1831,8 +1848,8 @@
   <conditionalFormatting sqref="M5:M11">
     <cfRule type="dataBar" priority="6">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1840,8 +1857,8 @@
   <conditionalFormatting sqref="O5:O6">
     <cfRule type="dataBar" priority="7">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1849,8 +1866,8 @@
   <conditionalFormatting sqref="Q5:Q6">
     <cfRule type="dataBar" priority="8">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1858,8 +1875,8 @@
   <conditionalFormatting sqref="S5:S6">
     <cfRule type="dataBar" priority="9">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1867,8 +1884,8 @@
   <conditionalFormatting sqref="U5:U6">
     <cfRule type="dataBar" priority="10">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>
@@ -1876,8 +1893,8 @@
   <conditionalFormatting sqref="W5:W6">
     <cfRule type="dataBar" priority="11">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FF638EC6"/>
       </dataBar>
     </cfRule>

</xml_diff>